<commit_message>
Update Appendix B Class D table
</commit_message>
<xml_diff>
--- a/data/criteria_ratios_20230315.xlsx
+++ b/data/criteria_ratios_20230315.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ltimaofile01.limno.com\Projects\DDOEIP\Water Quality Program Update\Impairment Assessment Updates\ImpairmentReview_2020\Analysis_Fall_2022\reference_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5BA280-D0A6-4C37-875F-012B2FC87408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E24ABF-615B-45D2-88D6-67DCC04C3192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-4575" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{F3D8D3B5-76FB-40F3-B3A3-06412D07EB80}"/>
   </bookViews>
   <sheets>
     <sheet name="Tim's Table" sheetId="1" r:id="rId1"/>
-    <sheet name="Lookup Table" sheetId="2" r:id="rId2"/>
+    <sheet name="Lookup Table" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="118">
   <si>
     <t>Pollutant</t>
   </si>
@@ -365,6 +365,30 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>NA - all results detected</t>
+  </si>
+  <si>
+    <t>ccc_dl_ratio_range</t>
+  </si>
+  <si>
+    <t>cmc_dl_ratio_range</t>
+  </si>
+  <si>
+    <t>d_dl_ratio_range</t>
+  </si>
+  <si>
+    <t>d_criterion</t>
+  </si>
+  <si>
+    <t>cmc_criterion</t>
+  </si>
+  <si>
+    <t>ccc_criterion</t>
+  </si>
+  <si>
+    <t>waterbody-specific</t>
   </si>
 </sst>
 </file>
@@ -405,7 +429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,18 +488,20 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -801,7 +827,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,10 +836,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="15" t="s">
@@ -822,19 +848,19 @@
       <c r="D1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>49</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>24</v>
       </c>
       <c r="J1" s="17" t="s">
@@ -1588,7 +1614,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="13" t="s">
+      <c r="A28" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1602,219 +1628,475 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B045A08E-C997-4A83-98AC-8A1F321FFF74}">
-  <dimension ref="A1:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D18487C-A8AE-4BF0-84B7-FFBA18A4F2CC}">
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>81</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="H1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
-        <v>107</v>
+      <c r="B2">
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E2">
+        <v>340</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
-      <c r="B3" t="s">
-        <v>108</v>
+      <c r="B3">
+        <v>4.3E-3</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>2.4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3">
+        <v>3.2000000000000003E-4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
-      <c r="B4" t="s">
-        <v>107</v>
+      <c r="B4">
+        <v>10.76</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E4">
+        <v>16.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
-        <v>108</v>
+      <c r="B5">
+        <v>1E-3</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5">
+        <v>1.2E-4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>85</v>
       </c>
-      <c r="B6" t="s">
-        <v>108</v>
+      <c r="B6">
+        <v>1E-3</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6">
+        <v>1.8E-5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>86</v>
       </c>
-      <c r="B7" t="s">
-        <v>108</v>
+      <c r="B7">
+        <v>1E-3</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>87</v>
       </c>
-      <c r="B8" t="s">
-        <v>107</v>
+      <c r="B8">
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>62</v>
       </c>
       <c r="D8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E8">
+        <v>0.24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H8">
+        <v>1.1999999999999999E-6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>88</v>
       </c>
-      <c r="B9" t="s">
-        <v>108</v>
+      <c r="B9">
+        <v>3.8E-3</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H9">
+        <v>3.1999999999999999E-5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
-      <c r="B11" t="s">
-        <v>107</v>
+      <c r="B11">
+        <v>0.77</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>1.4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11">
+        <v>0.15</v>
+      </c>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>91</v>
       </c>
-      <c r="B12" t="s">
-        <v>109</v>
+      <c r="B12">
+        <v>1.4E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12">
+        <v>6.3999999999999997E-5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>92</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="D13" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13">
+        <v>26000</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
-      <c r="B14" t="s">
-        <v>107</v>
+      <c r="B14">
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14">
+        <v>90</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>95</v>
       </c>
@@ -1825,24 +2107,60 @@
         <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E15" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15">
+        <v>70</v>
+      </c>
+      <c r="I15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>93</v>
       </c>
-      <c r="B16" t="s">
-        <v>107</v>
+      <c r="B16">
+        <v>600</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E16" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1853,10 +2171,28 @@
         <v>109</v>
       </c>
       <c r="D17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>109</v>
+      </c>
+      <c r="H17">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1867,24 +2203,60 @@
         <v>109</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18">
+        <v>0.13</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>98</v>
       </c>
-      <c r="B19" t="s">
-        <v>107</v>
+      <c r="B19">
+        <v>400</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="D19" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" t="s">
+        <v>109</v>
+      </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1895,10 +2267,28 @@
         <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20">
+        <v>30</v>
+      </c>
+      <c r="I20" t="s">
+        <v>40</v>
+      </c>
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -1909,10 +2299,28 @@
         <v>109</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="I21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1923,10 +2331,28 @@
         <v>109</v>
       </c>
       <c r="D22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" t="s">
+        <v>109</v>
+      </c>
+      <c r="H22">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>102</v>
       </c>
@@ -1937,10 +2363,28 @@
         <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1951,10 +2395,29 @@
         <v>109</v>
       </c>
       <c r="D24" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+      <c r="J24" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>